<commit_message>
forum yfir og loguðum notendagreyninguna
</commit_message>
<xml_diff>
--- a/documentation/notendagreining.xlsx
+++ b/documentation/notendagreining.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\runar\Desktop\verklegtnamskeid1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Fanna\OneDrive\Skjáborð\Assignments\Verknamið\verklegtnamskeid1\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43974C45-0D9C-4DFD-950C-CEC5015BC9AB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="67" documentId="13_ncr:1_{43974C45-0D9C-4DFD-950C-CEC5015BC9AB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{6968EE24-F509-48B8-A90C-521ADEDDF46D}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,61 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="37">
-  <si>
-    <t>Greining Notendahópa / User Group Analysis</t>
-  </si>
-  <si>
-    <t>Nafn hópsins/Name of the user group</t>
-  </si>
-  <si>
-    <t>Aldur/age</t>
-  </si>
-  <si>
-    <t>Kyn/gender</t>
-  </si>
-  <si>
-    <t>Menntun/Education</t>
-  </si>
-  <si>
-    <t>Hæfni, vanhæfni/Abilities, disabilities</t>
-  </si>
-  <si>
-    <t>Tölvufærni/General computer skills</t>
-  </si>
-  <si>
-    <t>Hversu oft/how often</t>
-  </si>
-  <si>
-    <t>Hversu lengi/for how long</t>
-  </si>
-  <si>
-    <t>Færni notenda/user skills</t>
-  </si>
-  <si>
-    <t>Fjöldi notenda/Number of users</t>
-  </si>
-  <si>
-    <t>AF HVERJU: Helstu notendamarkmið/ WHY: main user goals</t>
-  </si>
-  <si>
-    <t>HVAÐ: Tæknilegt umhverfi/ WHAT:Technical environment</t>
-  </si>
-  <si>
-    <t>HVAR: Raunverulegt umhverfi/ WHERE: The usage environment</t>
-  </si>
-  <si>
-    <t>HVERJIR: Bakgrunnur/ 
-WHO: background</t>
-  </si>
-  <si>
-    <t>HVENÆR: Notkun kerfis/ 
-WHEN:Usage of the software</t>
-  </si>
-  <si>
-    <t>HVERSU: Mikilvægur er hópurinn?/ 
-HOW: Important is this user group?</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="40">
   <si>
     <t>Öll</t>
   </si>
@@ -105,9 +51,6 @@
     <t xml:space="preserve"> 2 - 3</t>
   </si>
   <si>
-    <t>Skipuleggur ferðir, hvenær þær eru farnar og til hvaða áfangstaðar</t>
-  </si>
-  <si>
     <t>Dagleg notkun á vinnutíma</t>
   </si>
   <si>
@@ -145,6 +88,70 @@
   </si>
   <si>
     <t>Tölvureynsla og góð þekking</t>
+  </si>
+  <si>
+    <t>Skipuleggur ferðir, hvenær þær eru farnar og til hvaða áfangstaða</t>
+  </si>
+  <si>
+    <t>WHO</t>
+  </si>
+  <si>
+    <t>Notendamarkmið</t>
+  </si>
+  <si>
+    <t>WHY</t>
+  </si>
+  <si>
+    <t>Tæknilegt umhverfi</t>
+  </si>
+  <si>
+    <t>WHAT</t>
+  </si>
+  <si>
+    <t>Raunverulegt umhverfi</t>
+  </si>
+  <si>
+    <t>WHERE</t>
+  </si>
+  <si>
+    <t>WHEN</t>
+  </si>
+  <si>
+    <t>Hversu oft</t>
+  </si>
+  <si>
+    <t>Hversu lengi</t>
+  </si>
+  <si>
+    <t>Færni notenda</t>
+  </si>
+  <si>
+    <t>Aldur</t>
+  </si>
+  <si>
+    <t>Kyn</t>
+  </si>
+  <si>
+    <t>Menntun</t>
+  </si>
+  <si>
+    <t>Hæfni, vanhæfni</t>
+  </si>
+  <si>
+    <t>Tölvufærni</t>
+  </si>
+  <si>
+    <t>Fjöldi notenda</t>
+  </si>
+  <si>
+    <t>HOW:
+Hversu mikilvægur er hópurinn?</t>
+  </si>
+  <si>
+    <t>Nafn hópsins</t>
+  </si>
+  <si>
+    <t>Greining Notendahópa</t>
   </si>
 </sst>
 </file>
@@ -506,7 +513,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -520,23 +527,8 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -608,12 +600,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
@@ -623,8 +609,26 @@
     <xf numFmtId="16" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" indent="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -908,269 +912,275 @@
   <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="35.44140625" style="3" customWidth="1"/>
+    <col min="1" max="1" width="35.453125" style="3" customWidth="1"/>
     <col min="2" max="2" width="28" customWidth="1"/>
-    <col min="3" max="3" width="31.44140625" customWidth="1"/>
-    <col min="4" max="4" width="33.77734375" customWidth="1"/>
+    <col min="3" max="3" width="31.453125" customWidth="1"/>
+    <col min="4" max="4" width="33.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="18" x14ac:dyDescent="0.35">
-      <c r="A1" s="40" t="s">
+    <row r="1" spans="1:4" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A1" s="37" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+    </row>
+    <row r="2" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="3" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="33" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="13"/>
+      <c r="C4" s="13"/>
+      <c r="D4" s="14"/>
+    </row>
+    <row r="5" spans="1:4" ht="21.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="27" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5" s="28" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="28" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" s="29" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="21.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="27" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="41"/>
-      <c r="C1" s="41"/>
-    </row>
-    <row r="2" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="3" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="4" t="s">
+      <c r="C6" s="28" t="s">
+        <v>0</v>
+      </c>
+      <c r="D6" s="29" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="21.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="B7" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" s="29" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="24.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B8" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="C8" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="D8" s="16" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" s="18" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A10" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="B10" s="31" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" s="32" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A11" s="33" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" s="21"/>
+      <c r="C11" s="21"/>
+      <c r="D11" s="22"/>
+    </row>
+    <row r="12" spans="1:4" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A12" s="34" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C12" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="D12" s="20" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A13" s="33" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" s="21"/>
+      <c r="C13" s="21"/>
+      <c r="D13" s="22"/>
+    </row>
+    <row r="14" spans="1:4" s="6" customFormat="1" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A14" s="36" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14" s="39" t="s">
+        <v>17</v>
+      </c>
+      <c r="C14" s="39" t="s">
+        <v>17</v>
+      </c>
+      <c r="D14" s="40" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A15" s="33" t="s">
         <v>26</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="36.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" s="18"/>
-      <c r="C4" s="18"/>
-      <c r="D4" s="19"/>
-    </row>
-    <row r="5" spans="1:4" ht="21.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="32" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" s="33" t="s">
-        <v>20</v>
-      </c>
-      <c r="C5" s="33" t="s">
-        <v>20</v>
-      </c>
-      <c r="D5" s="34" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="21.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="32" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6" s="33" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" s="33" t="s">
-        <v>17</v>
-      </c>
-      <c r="D6" s="34" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="21.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="32" t="s">
-        <v>4</v>
-      </c>
-      <c r="B7" s="33" t="s">
-        <v>21</v>
-      </c>
-      <c r="C7" s="33" t="s">
-        <v>21</v>
-      </c>
-      <c r="D7" s="34" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="73.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="B8" s="20" t="s">
-        <v>18</v>
-      </c>
-      <c r="C8" s="20" t="s">
-        <v>18</v>
-      </c>
-      <c r="D8" s="21" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="39" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="17" t="s">
+      <c r="B15" s="21"/>
+      <c r="C15" s="21"/>
+      <c r="D15" s="22"/>
+    </row>
+    <row r="16" spans="1:4" ht="21.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B16" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="C16" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="D16" s="16" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A17" s="35" t="s">
+        <v>27</v>
+      </c>
+      <c r="B17" s="23"/>
+      <c r="C17" s="23"/>
+      <c r="D17" s="24"/>
+    </row>
+    <row r="18" spans="1:4" ht="26.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="B18" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="22" t="s">
-        <v>36</v>
-      </c>
-      <c r="C9" s="22" t="s">
-        <v>36</v>
-      </c>
-      <c r="D9" s="23" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="171" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="B10" s="38" t="s">
-        <v>22</v>
-      </c>
-      <c r="C10" s="24" t="s">
-        <v>22</v>
-      </c>
-      <c r="D10" s="39" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A11" s="5" t="s">
+      <c r="C18" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="D18" s="16" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="23.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="B19" s="28" t="s">
+        <v>1</v>
+      </c>
+      <c r="C19" s="30" t="s">
+        <v>1</v>
+      </c>
+      <c r="D19" s="29" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="23.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A20" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="B20" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="C20" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="D20" s="16" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A21" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="B21" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="C21" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="26"/>
-      <c r="C11" s="26"/>
-      <c r="D11" s="27"/>
-    </row>
-    <row r="12" spans="1:4" ht="103.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="6"/>
-      <c r="B12" s="24" t="s">
-        <v>23</v>
-      </c>
-      <c r="C12" s="24" t="s">
-        <v>27</v>
-      </c>
-      <c r="D12" s="25" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A13" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B13" s="26"/>
-      <c r="C13" s="26"/>
-      <c r="D13" s="27"/>
-    </row>
-    <row r="14" spans="1:4" s="11" customFormat="1" ht="28.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="10"/>
-      <c r="B14" s="35" t="s">
-        <v>35</v>
-      </c>
-      <c r="C14" s="35" t="s">
-        <v>35</v>
-      </c>
-      <c r="D14" s="36" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A15" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B15" s="26"/>
-      <c r="C15" s="26"/>
-      <c r="D15" s="27"/>
-    </row>
-    <row r="16" spans="1:4" ht="56.55" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="8"/>
-      <c r="B16" s="20" t="s">
-        <v>28</v>
-      </c>
-      <c r="C16" s="20" t="s">
-        <v>28</v>
-      </c>
-      <c r="D16" s="21" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A17" s="7" t="s">
+      <c r="D21" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="B17" s="28"/>
-      <c r="C17" s="28"/>
-      <c r="D17" s="29"/>
-    </row>
-    <row r="18" spans="1:4" ht="67.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="B18" s="20" t="s">
-        <v>24</v>
-      </c>
-      <c r="C18" s="20" t="s">
-        <v>24</v>
-      </c>
-      <c r="D18" s="21" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="23.55" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="15" t="s">
-        <v>8</v>
-      </c>
-      <c r="B19" s="33" t="s">
-        <v>18</v>
-      </c>
-      <c r="C19" s="37" t="s">
-        <v>18</v>
-      </c>
-      <c r="D19" s="34" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="63.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="B20" s="20" t="s">
-        <v>18</v>
-      </c>
-      <c r="C20" s="20" t="s">
-        <v>18</v>
-      </c>
-      <c r="D20" s="21" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="117.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="B21" s="30" t="s">
-        <v>25</v>
-      </c>
-      <c r="C21" s="30" t="s">
-        <v>29</v>
-      </c>
-      <c r="D21" s="31" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="32.4" x14ac:dyDescent="0.3">
-      <c r="A22" s="9"/>
-    </row>
-    <row r="23" spans="1:4" ht="32.4" x14ac:dyDescent="0.3">
-      <c r="A23" s="9"/>
-    </row>
-    <row r="24" spans="1:4" ht="32.4" x14ac:dyDescent="0.3">
-      <c r="A24" s="9"/>
-    </row>
-    <row r="25" spans="1:4" ht="32.4" x14ac:dyDescent="0.3">
-      <c r="A25" s="9"/>
-    </row>
-    <row r="26" spans="1:4" ht="32.4" x14ac:dyDescent="0.3">
-      <c r="A26" s="9"/>
+    </row>
+    <row r="22" spans="1:4" ht="32" x14ac:dyDescent="0.35">
+      <c r="A22" s="5"/>
+    </row>
+    <row r="23" spans="1:4" ht="32" x14ac:dyDescent="0.35">
+      <c r="A23" s="5"/>
+    </row>
+    <row r="24" spans="1:4" ht="32" x14ac:dyDescent="0.35">
+      <c r="A24" s="5"/>
+    </row>
+    <row r="25" spans="1:4" ht="32" x14ac:dyDescent="0.35">
+      <c r="A25" s="5"/>
+    </row>
+    <row r="26" spans="1:4" ht="32" x14ac:dyDescent="0.35">
+      <c r="A26" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>